<commit_message>
Add multi-strain workflow basics
</commit_message>
<xml_diff>
--- a/data/e_coli_genomes/lab_strains.xlsx
+++ b/data/e_coli_genomes/lab_strains.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cam/Projects/bitome/data/e_coli_genomes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91E9630-9B6B-B649-B20D-D1259403C211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE9DAC2-5555-134B-BA82-8E5703B83503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{CD230B44-24BB-4D3C-917A-94690026C49F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>patric_id</t>
   </si>
@@ -138,13 +138,61 @@
   </si>
   <si>
     <t>042</t>
+  </si>
+  <si>
+    <t>CFT073</t>
+  </si>
+  <si>
+    <t>Escherichia coli Cft073</t>
+  </si>
+  <si>
+    <t>InPec: UPEC</t>
+  </si>
+  <si>
+    <t>AE014075</t>
+  </si>
+  <si>
+    <t>Escherichia coli UMN026</t>
+  </si>
+  <si>
+    <t>UMN026</t>
+  </si>
+  <si>
+    <t>CU928163</t>
+  </si>
+  <si>
+    <t>AE014073</t>
+  </si>
+  <si>
+    <t>Shigella flexneri 2a str. 2457T</t>
+  </si>
+  <si>
+    <t>Shigella 2457T</t>
+  </si>
+  <si>
+    <t>CP000970</t>
+  </si>
+  <si>
+    <t>Escherichia coli SMS-3-5</t>
+  </si>
+  <si>
+    <t>SMS-3-5</t>
+  </si>
+  <si>
+    <t>CP000946</t>
+  </si>
+  <si>
+    <t>Escherichia coli ATCC 8739</t>
+  </si>
+  <si>
+    <t>ATCC 8739</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +212,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -195,6 +251,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92350CB0-C2D3-4838-98DB-BBE66C5AD74F}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -693,6 +750,88 @@
         <v>11</v>
       </c>
     </row>
+    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>199310.4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>585056.69999999995</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>198215.6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>439855.1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>481805.6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
     <sortCondition ref="E1"/>

</xml_diff>